<commit_message>
Additions to Word file sec. B.2 transferred to Excel file, too.
</commit_message>
<xml_diff>
--- a/V3.1.1/Mapping_Table_Excel_xMCF_STEP.xlsx
+++ b/V3.1.1/Mapping_Table_Excel_xMCF_STEP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MWEINERT\Documents\05 FAT\04 UAKs\01 UAK MCF\000000 ISO Docs &amp; Guidelines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Franke\Kunden\VDA-AK_25\xMCF_at_GitHub\createXSDforxMCF\V3.1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00459567-7750-4C3D-9355-BA0DB7DEBB92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EB03A2-D00B-4029-A915-EEC39DD11CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60600" yWindow="330" windowWidth="23940" windowHeight="16275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Comments</t>
   </si>
@@ -104,6 +104,21 @@
   </si>
   <si>
     <t>xMCF is Master; STEP parameter to be ignored to avoid conflicts</t>
+  </si>
+  <si>
+    <t>unit system used by the file</t>
+  </si>
+  <si>
+    <t>date on which the file is created</t>
+  </si>
+  <si>
+    <t>version code of the standard used</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>DateTimeAssignment</t>
   </si>
 </sst>
 </file>
@@ -667,7 +682,7 @@
   <dimension ref="A7:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,12 +947,16 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
+      <c r="K23" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -947,12 +966,16 @@
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="2"/>
+      <c r="F24" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="K24" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
@@ -967,7 +990,9 @@
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
+      <c r="K25" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Excel file, matching previous update of Word file.
</commit_message>
<xml_diff>
--- a/V3.1.1/Mapping_Table_Excel_xMCF_STEP.xlsx
+++ b/V3.1.1/Mapping_Table_Excel_xMCF_STEP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Franke\Kunden\VDA-AK_25\xMCF_at_GitHub\createXSDforxMCF\V3.1.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franke\Documents\PROSTEP\Kunden\VDA-AK_25\xMCF_at_GitHub\createXSDforxMCF\V3.1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EB03A2-D00B-4029-A915-EEC39DD11CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D89856-9950-4E07-9872-7DD38D0AB95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60600" yWindow="330" windowWidth="23940" windowHeight="16275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57810" yWindow="165" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Comments</t>
   </si>
@@ -57,16 +57,9 @@
     <t>&lt;version/&gt;</t>
   </si>
   <si>
-    <t>&lt;loc&gt; in xMCF can be used nested inside the actual connection type (e.g. spotweld) or directly nested in &lt;connection_0d/&gt; on the same level as &lt;spotweld/&gt;</t>
-  </si>
-  <si>
     <t>MatingDefinition</t>
   </si>
   <si>
-    <t xml:space="preserve">Step defines the connection type as attribute within MatedPartRelationship
-“connection_[012]d_type” is just a placeholder for a specific name, i.e. “spotweld”, “rivet”, … </t>
-  </si>
-  <si>
     <t>MatedPartAssociation</t>
   </si>
   <si>
@@ -97,35 +90,61 @@
     <t>MatingType</t>
   </si>
   <si>
-    <t>STEP (xml representation)</t>
-  </si>
-  <si>
-    <t>xMCF (xml representation)</t>
-  </si>
-  <si>
-    <t>xMCF is Master; STEP parameter to be ignored to avoid conflicts</t>
-  </si>
-  <si>
-    <t>unit system used by the file</t>
-  </si>
-  <si>
-    <t>date on which the file is created</t>
-  </si>
-  <si>
-    <t>version code of the standard used</t>
-  </si>
-  <si>
     <t>Unit</t>
   </si>
   <si>
-    <t>DateTimeAssignment</t>
+    <t>No corresponding entity in ISO 10303-242.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MatingDefinition points to part version of assembly, which is irrelevant for χMCF. Hence, there is no correlation between both XML elements. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MatedPartAssociation contains transformation, hence is necessary. 
+List of part codes is mandatory within it. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semantics of both XML elements 
+does not match exactly. They are just similar. 
+MatedPartRelationship is not relevant for χMCF use cases. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISO 10303-242 defines the connection type as attribute within MatedPartRelationship, which is not relevant (see above). 
+“connection_[012]d_type” is just a placeholder for a specific name, i.e. “spotweld”, “rivet”,”seamweld”, …  </t>
+  </si>
+  <si>
+    <t>&lt;loc/&gt; in χMCF is nested in &lt;connection_[012]d/&gt;. 
+ISO 10303-242 entity is not relevant, since χMCF is master for location.</t>
+  </si>
+  <si>
+    <t>χMCF (xml representation)</t>
+  </si>
+  <si>
+    <t>χMCF is Master; STEP parameter to be ignored to avoid conflicts</t>
+  </si>
+  <si>
+    <t>ISO 10303-242 (xml representation)</t>
+  </si>
+  <si>
+    <t>Unit system used by the file. However, they do not need to be coincident (e.g., one could be in m, the other one in inches).</t>
+  </si>
+  <si>
+    <t>TimeStamp in header element</t>
+  </si>
+  <si>
+    <t>Date on which the file is created. Does not need to be coincident.</t>
+  </si>
+  <si>
+    <t>Encoded in XML name space</t>
+  </si>
+  <si>
+    <t>Version code of the standard used. These XML elements are not related.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +166,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -156,7 +181,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -170,24 +195,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -328,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -336,22 +343,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -366,38 +367,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -679,329 +689,349 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A7:K25"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A7:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="5.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="1" customWidth="1"/>
-    <col min="6" max="9" width="5.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="45.7109375" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="5" width="5.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7" max="10" width="5.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="45.7109375" style="19" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="16" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="12" t="s">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="12" t="s">
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="12" t="s">
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-    </row>
-    <row r="14" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="22" t="s">
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="11"/>
+    </row>
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3" t="s">
+      <c r="F16" s="10"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3" t="s">
+    </row>
+    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="5" t="s">
+      <c r="G17" s="8"/>
+      <c r="H17" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="3" t="s">
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="11"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="11"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="11"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="11"/>
+    </row>
+    <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8" t="s">
-        <v>28</v>
+      <c r="J24" s="3"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="22" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G15:J15"/>
+  <mergeCells count="5">
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="G10:K10"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="74" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;8&amp;F&amp;R&amp;8&amp;D</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>